<commit_message>
Hyperlink to appropriate add-in.
</commit_message>
<xml_diff>
--- a/xll_math.xlsx
+++ b/xll_math.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23704"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalx\source\repos\xlladdins\xll_math\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalx\source\repos\xlladdins\xll_math\x64\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29234427-AEC8-459A-B5CB-D35843BC5080}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB639A9B-44E6-42F5-B656-CF10CB9DF48F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="2730" windowWidth="20595" windowHeight="13215" xr2:uid="{981A9639-7D1C-4678-9EFA-5818ABE27987}"/>
+    <workbookView xWindow="4605" yWindow="1725" windowWidth="20595" windowHeight="13215" xr2:uid="{445382C7-F62C-4488-81C7-3D9667030E50}"/>
   </bookViews>
   <sheets>
     <sheet name="XLL_MATH" sheetId="1" r:id="rId1"/>
@@ -705,7 +705,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -730,9 +730,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -765,8 +781,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -777,14 +794,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1164,7 +1182,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB73EE4-1EBE-4A92-AF8A-63D4F6C3CC32}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4220C78-80A9-484D-8291-57E03B482177}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:C59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
@@ -1177,8 +1196,8 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="str">
-        <f>HYPERLINK("https://xlladdins.com/addins/xll_math.xll", "XLL_MATH")</f>
+      <c r="B2" s="7" t="str" cm="1">
+        <f t="array" ref="B2">HYPERLINK("https://xlladdins.com/addins/xll_math" &amp; WinXX() &amp; ".xll", "XLL_MATH")</f>
         <v>XLL_MATH</v>
       </c>
       <c r="C2" t="s">
@@ -1186,7 +1205,7 @@
       </c>
     </row>
     <row r="4" spans="2:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>170</v>
       </c>
     </row>
@@ -1194,7 +1213,7 @@
       <c r="B6" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>166</v>
       </c>
     </row>
@@ -1202,7 +1221,7 @@
       <c r="B7" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>163</v>
       </c>
     </row>
@@ -1210,7 +1229,7 @@
       <c r="B8" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>161</v>
       </c>
     </row>
@@ -1218,7 +1237,7 @@
       <c r="B9" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1226,7 +1245,7 @@
       <c r="B10" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>156</v>
       </c>
     </row>
@@ -1234,7 +1253,7 @@
       <c r="B11" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>153</v>
       </c>
     </row>
@@ -1242,7 +1261,7 @@
       <c r="B12" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1250,7 +1269,7 @@
       <c r="B13" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>148</v>
       </c>
     </row>
@@ -1258,7 +1277,7 @@
       <c r="B14" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>146</v>
       </c>
     </row>
@@ -1266,7 +1285,7 @@
       <c r="B15" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1274,7 +1293,7 @@
       <c r="B16" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1282,7 +1301,7 @@
       <c r="B17" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>138</v>
       </c>
     </row>
@@ -1290,7 +1309,7 @@
       <c r="B18" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>136</v>
       </c>
     </row>
@@ -1298,7 +1317,7 @@
       <c r="B19" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>133</v>
       </c>
     </row>
@@ -1306,7 +1325,7 @@
       <c r="B20" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1314,7 +1333,7 @@
       <c r="B21" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1322,7 +1341,7 @@
       <c r="B22" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1330,7 +1349,7 @@
       <c r="B23" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1338,7 +1357,7 @@
       <c r="B24" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1346,7 +1365,7 @@
       <c r="B25" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="6" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1354,7 +1373,7 @@
       <c r="B26" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="5" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1362,7 +1381,7 @@
       <c r="B27" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1370,7 +1389,7 @@
       <c r="B28" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="5" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1378,7 +1397,7 @@
       <c r="B29" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="6" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1386,7 +1405,7 @@
       <c r="B30" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="5" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1394,7 +1413,7 @@
       <c r="B31" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="6" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1402,7 +1421,7 @@
       <c r="B32" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="5" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1410,7 +1429,7 @@
       <c r="B33" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="6" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1418,7 +1437,7 @@
       <c r="B34" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="5" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1426,7 +1445,7 @@
       <c r="B35" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="6" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1434,7 +1453,7 @@
       <c r="B36" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1442,7 +1461,7 @@
       <c r="B37" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="6" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1450,7 +1469,7 @@
       <c r="B38" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1458,7 +1477,7 @@
       <c r="B39" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="6" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1466,7 +1485,7 @@
       <c r="B40" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="5" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1474,7 +1493,7 @@
       <c r="B41" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="6" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1482,7 +1501,7 @@
       <c r="B42" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="5" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1490,7 +1509,7 @@
       <c r="B43" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="6" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1498,7 +1517,7 @@
       <c r="B44" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="5" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1506,7 +1525,7 @@
       <c r="B45" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="6" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1514,7 +1533,7 @@
       <c r="B46" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1522,7 +1541,7 @@
       <c r="B47" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="6" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1530,7 +1549,7 @@
       <c r="B48" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1538,7 +1557,7 @@
       <c r="B49" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C49" s="6" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1546,7 +1565,7 @@
       <c r="B50" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C50" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1554,7 +1573,7 @@
       <c r="B51" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C51" s="6" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1562,7 +1581,7 @@
       <c r="B52" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C52" s="5" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1570,7 +1589,7 @@
       <c r="B53" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1578,7 +1597,7 @@
       <c r="B54" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="5" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1586,7 +1605,7 @@
       <c r="B55" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C55" s="6" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1594,7 +1613,7 @@
       <c r="B56" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C56" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1602,7 +1621,7 @@
       <c r="B57" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C57" s="6" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1610,7 +1629,7 @@
       <c r="B58" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C58" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1618,7 +1637,7 @@
       <c r="B59" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C59" s="6" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1628,7 +1647,8 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{193FF19A-B112-4597-9172-9BDAC1EDB595}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69A6F21-1A3C-4F9E-9A6E-AB13618F716F}">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -1670,7 +1690,8 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{208C0A75-7E39-4FE8-8C51-6AE92DB7B1B8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4D520E8-2BB9-4B10-9AA0-1048B2689E2C}">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -1720,7 +1741,8 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89723C1B-8F49-4414-98CC-32EF07FE492B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11352063-4F58-48CA-AEDA-D861A1DB2E12}">
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -1762,7 +1784,8 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31F6EDF0-4EFF-42F5-A5FC-D2040707287A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD8E9BA0-4E7B-432B-A390-D73750F02570}">
+  <sheetPr codeName="Sheet13"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -1804,7 +1827,8 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA3DA9F-5B1A-4A47-8DB8-B8B7D4861255}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{813EF715-57DA-42F6-8061-746ED0AFD276}">
+  <sheetPr codeName="Sheet14"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -1846,7 +1870,8 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E0459C0-9C6A-4126-B94E-DC794AF7D29A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F938C582-276C-42B2-AC60-F8C9A3844471}">
+  <sheetPr codeName="Sheet15"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -1888,7 +1913,8 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C0B0AB-786F-4871-B50E-AC96815FF64E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0F61301-6C71-42B7-BAAD-902CBF66FE36}">
+  <sheetPr codeName="Sheet16"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -1930,7 +1956,8 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A44D7C-4CD2-4D40-BDF3-BA45DA7347C6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63CFC0ED-D070-4139-933A-C1D8EFF2DD4E}">
+  <sheetPr codeName="Sheet17"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -1972,7 +1999,8 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63EE9101-18C7-4327-BF6E-AEB13022762C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5768E982-1DD0-45F1-BB49-004AC19B31D3}">
+  <sheetPr codeName="Sheet18"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2014,7 +2042,8 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BD0E346-360B-4782-97F4-08D35B5F7B00}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14079143-9AAC-4BEF-8906-DAA7E583655E}">
+  <sheetPr codeName="Sheet19"/>
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2064,7 +2093,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6163D1-90A9-4F57-8658-4C96833C0E96}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F201FBC3-0CCA-41B5-A568-147AB9C1D6C0}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2106,7 +2136,8 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE5F619-7D2C-44A2-8D6C-66BD9965BFCB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E91F2935-5DA7-44CE-9972-147B87FF5D78}">
+  <sheetPr codeName="Sheet20"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2148,7 +2179,8 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47601CB4-D714-4E09-A1D5-029063551B86}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35733D25-D493-4615-A1FE-B54AA47FB1D6}">
+  <sheetPr codeName="Sheet21"/>
   <dimension ref="B2:D8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2206,7 +2238,8 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2CEC020-AD17-4A3F-85CC-40DFD8A25141}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C5FD0FA-F95B-498C-9955-3EEF0306923C}">
+  <sheetPr codeName="Sheet22"/>
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2256,7 +2289,8 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8DE694E-0035-4DC5-8ABC-CBB8C76C7220}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31FD76F5-FCD5-4539-80A1-CA1B986C1452}">
+  <sheetPr codeName="Sheet23"/>
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2306,7 +2340,8 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B04A7A-5D51-4120-8E71-A55F3A130648}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD9EC15-2126-4C0B-87D7-C0D4C0684EF0}">
+  <sheetPr codeName="Sheet24"/>
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2356,7 +2391,8 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{372047AB-A48F-43C2-8F37-721314347D41}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73CE6FC6-A265-4AA4-8DD3-12F871E72422}">
+  <sheetPr codeName="Sheet25"/>
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2406,7 +2442,8 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FDA01E6-2CF3-4F9D-9004-289D40F57368}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D6ABC7-BDAC-42EB-B9FF-12DE7FDC4C76}">
+  <sheetPr codeName="Sheet26"/>
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2456,7 +2493,8 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629AA14B-D10B-4FB2-91B7-5710DCDC4392}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57ACC43F-2F50-4F15-8D63-DCB1A1C94D3A}">
+  <sheetPr codeName="Sheet27"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2498,7 +2536,8 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13617D8F-807F-4F3D-B5DD-9EA159FAC34D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B10805FB-3D6D-44AF-9E18-25710E4496AC}">
+  <sheetPr codeName="Sheet28"/>
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2548,7 +2587,8 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAFF70A7-C690-42AC-9D7A-791FD88D7E92}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C92D25F-DA46-40E7-BBC8-EF29B4C12B43}">
+  <sheetPr codeName="Sheet29"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2590,7 +2630,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282B9D4D-D03A-4C2C-BC4A-B58E4E0C335E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C09E223-3FEC-4DE5-B376-1CF007F1D36C}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2632,7 +2673,8 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F1E689D-CB15-4315-9E8C-D90E6EC1D330}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{431FC9F1-4BB2-4109-8080-2FBC937E056D}">
+  <sheetPr codeName="Sheet30"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2674,7 +2716,8 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4EE49B2-3647-4ACF-8D4C-225BBF816FE6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C811DA5F-6AA4-4016-BAED-1F220DD76FC8}">
+  <sheetPr codeName="Sheet31"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2716,7 +2759,8 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D0470B1-D815-49EF-8782-2219CD5845F9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0157FC3-8318-48EF-BBC6-2EA2B429F6A2}">
+  <sheetPr codeName="Sheet32"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2758,7 +2802,8 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6C0AF0-0D60-4740-BAAE-382844C69C57}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC0C464E-4B49-44A7-A987-7CE85331F187}">
+  <sheetPr codeName="Sheet33"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2800,7 +2845,8 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6104B084-F946-479D-B6B1-85C8B9B592A7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{006B0079-00E0-404A-B6E6-78B46252E42E}">
+  <sheetPr codeName="Sheet34"/>
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2850,7 +2896,8 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF9A8E6B-6DDC-431F-AF24-0E0141C71A74}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C274B6B-41E2-4864-89D2-C9926F082176}">
+  <sheetPr codeName="Sheet35"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2892,7 +2939,8 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96B5FA1-0A55-48B6-B4EA-233E42D07562}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF9A8945-A099-4237-B6AE-C0895560B75A}">
+  <sheetPr codeName="Sheet36"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2934,7 +2982,8 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12D08A7C-4883-48C1-ABA7-36E38FBAAFF1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B454D3A4-767A-417D-862A-6E6BDFF785DA}">
+  <sheetPr codeName="Sheet37"/>
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2984,7 +3033,8 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B54CF128-AD2B-48B6-BF9B-CC776C5F6E27}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E2AD21-5A26-4462-B498-DC61352BC167}">
+  <sheetPr codeName="Sheet38"/>
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3034,7 +3084,8 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D770639E-4F32-407E-BB28-6810002773A3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0DD1669-4E70-44A0-A1D9-3164460EE8BA}">
+  <sheetPr codeName="Sheet39"/>
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3084,7 +3135,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AB88866-A7EA-431E-B81A-BA8BB750ABCB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA45E6A-7137-4D2F-9624-5201C4AD5287}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3126,7 +3178,8 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42BA023F-E52B-4347-9CDF-96F5B2F6915C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6108737E-92E8-4C3E-A58E-A9B36304B54E}">
+  <sheetPr codeName="Sheet40"/>
   <dimension ref="B2:D8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3184,7 +3237,8 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{745526FF-9FB2-4A04-B573-26EB89F99253}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8CD6203-4495-47B2-B1B0-E61628C8CE0B}">
+  <sheetPr codeName="Sheet41"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3226,7 +3280,8 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DFC1D29-2D4A-48A5-821F-B05596A4C7AE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{907A57E1-C577-4F8A-B951-926ACE4722F0}">
+  <sheetPr codeName="Sheet42"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3268,7 +3323,8 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{472129FB-D57C-4034-80CE-5A7EB87C3CEB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE85053-D9AE-40B6-9158-B501DF96978B}">
+  <sheetPr codeName="Sheet43"/>
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3318,7 +3374,8 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEEAEA86-EAE3-45FA-9B5A-1404DC324B2F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C3755DF-1B17-4AE5-A6A9-6AC5FA395267}">
+  <sheetPr codeName="Sheet44"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3360,7 +3417,8 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BDA5C37-857A-4768-AEB9-D2AE35940E02}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CDF70BD-C675-4670-AB38-7AE75397FA3E}">
+  <sheetPr codeName="Sheet45"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3402,7 +3460,8 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F8C1AEF-882D-4DCD-8C58-B9754CBDE514}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C94596F-4645-4B11-8040-856F2E8C53FF}">
+  <sheetPr codeName="Sheet46"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3444,7 +3503,8 @@
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8F22D0-0FD4-4546-AD62-33DF62D18DB2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DBC6D1A-1696-4CE1-BF5E-3685B554F3A4}">
+  <sheetPr codeName="Sheet47"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3486,7 +3546,8 @@
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064CA4DF-3123-44EB-80B0-20B54E1FE0ED}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A914AA6F-DBE4-4980-A903-80FD1E03C6BC}">
+  <sheetPr codeName="Sheet48"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3528,7 +3589,8 @@
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4227E47F-213A-4F56-9F86-151E6AE892A7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83CD6D89-F4C7-4BCA-89D1-CF4BAB7FF21F}">
+  <sheetPr codeName="Sheet49"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3570,7 +3632,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7205BA4-C1D3-446F-934E-AEF55A8667A4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D02D14C-4579-4B86-8267-C3A1C585063A}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3612,7 +3675,8 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3702274-EB23-42B8-B61F-D4B8FFB177A5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CD1CB5A-BA58-482C-A3DF-573D51314D27}">
+  <sheetPr codeName="Sheet50"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3654,7 +3718,8 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81DC52F3-E926-44AC-A847-4DA1C3A2AF57}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF62384-D894-4B6B-8323-75F77D092737}">
+  <sheetPr codeName="Sheet51"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3696,7 +3761,8 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B72120A0-5C94-43FD-8A3C-F7F458138446}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18B4709-9CFE-413D-812A-45E6A1B6835C}">
+  <sheetPr codeName="Sheet52"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3738,7 +3804,8 @@
 </file>
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C284DD-1D91-4151-84ED-A3492FA51CE0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DACFD242-B7DB-4EBD-92F4-4F240023089E}">
+  <sheetPr codeName="Sheet53"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3780,7 +3847,8 @@
 </file>
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A6CAB6-4250-4B62-B810-347294348F34}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946F1504-FD0C-4FB4-BAC4-9C39408E4C1A}">
+  <sheetPr codeName="Sheet54"/>
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3830,7 +3898,8 @@
 </file>
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C206837-8487-42B6-9408-FB96B19DB372}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C4D5C0A-6657-4DF0-94B2-3BF5BAD8280D}">
+  <sheetPr codeName="Sheet55"/>
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3881,7 +3950,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84240E25-36E3-46EC-97AA-D5E968DE6F25}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA044FF9-01CA-4BAF-9422-D3AFAB1B1E70}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3923,7 +3993,8 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF77050A-A19C-4927-82DF-0B84D0333ECF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3084C46-6AA0-4943-9FEB-5750FDBFE9C7}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3965,7 +4036,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53BACF8-60B1-487F-ADEC-82D999FF07B1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0E7FEDF-693C-4710-AB8B-5C711E695EFB}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4007,7 +4079,8 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63233417-19EF-491D-9D46-D10E23E75162}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{287DCFC9-87DA-49BB-A191-4C0406D4194B}">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">

</xml_diff>